<commit_message>
part III Adjacency/Target Tests
</commit_message>
<xml_diff>
--- a/CTestFiles/ourBoard.xlsx
+++ b/CTestFiles/ourBoard.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daria\Desktop\School\Software Engineering\Clue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daria\Desktop\School\Software Engineering\Clue\CluePaths\CTestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1C0BB1-040D-45D0-A354-88E3B4AEF253}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A32626-D42B-459B-B451-9E215FCE92BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{191238FF-631C-440F-96FB-A985FBB50CB5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="39">
   <si>
     <t>K</t>
   </si>
@@ -94,6 +94,60 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Light Blue</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Light Purple</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Closet</t>
+  </si>
+  <si>
+    <t>Doorway</t>
+  </si>
+  <si>
+    <t>Walkway</t>
+  </si>
+  <si>
+    <t>Test Targets</t>
+  </si>
+  <si>
+    <t>Adjacency List Test: Inside Room</t>
+  </si>
+  <si>
+    <t>Adjacency List Test: Walkways</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests: Doors</t>
+  </si>
+  <si>
+    <t>Adjacency List Test: Outside Door</t>
   </si>
 </sst>
 </file>
@@ -109,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +194,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -153,12 +237,46 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -167,6 +285,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC00CC"/>
+      <color rgb="FFFF99CC"/>
+      <color rgb="FFF480EE"/>
       <color rgb="FFA50021"/>
     </mruColors>
   </colors>
@@ -478,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{053D986D-1B28-4ED8-AF2F-62481DF0EE07}">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +611,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -532,7 +653,7 @@
       <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -567,7 +688,7 @@
       <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -585,7 +706,7 @@
       <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -733,7 +854,7 @@
       <c r="P4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -750,7 +871,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -777,7 +898,7 @@
       <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -804,7 +925,7 @@
       <c r="R5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="S5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="T5" s="2" t="s">
@@ -845,7 +966,7 @@
       <c r="J6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -880,7 +1001,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1002,7 +1123,7 @@
       <c r="S8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="T8" s="9" t="s">
         <v>8</v>
       </c>
       <c r="U8">
@@ -1090,10 +1211,10 @@
       <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="3" t="s">
@@ -1185,7 +1306,7 @@
       <c r="O11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="Q11" s="2" t="s">
@@ -1241,7 +1362,7 @@
       <c r="L12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N12" s="3" t="s">
@@ -1250,7 +1371,7 @@
       <c r="O12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="P12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q12" s="2" t="s">
@@ -1315,7 +1436,7 @@
       <c r="O13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="P13" s="8" t="s">
         <v>8</v>
       </c>
       <c r="Q13" s="3" t="s">
@@ -1335,7 +1456,7 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1424,7 +1545,7 @@
       <c r="H15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -1451,7 +1572,7 @@
       <c r="Q15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="R15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="S15" s="2" t="s">
@@ -1474,7 +1595,7 @@
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1495,10 +1616,10 @@
       <c r="J16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="K16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="7" t="s">
         <v>10</v>
       </c>
       <c r="M16" s="2" t="s">
@@ -1516,7 +1637,7 @@
       <c r="Q16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R16" s="4" t="s">
+      <c r="R16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="S16" s="2" t="s">
@@ -1672,7 +1793,7 @@
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -1752,7 +1873,7 @@
       <c r="I20" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K20" s="3" t="s">
@@ -1770,7 +1891,7 @@
       <c r="O20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="P20" s="9" t="s">
         <v>8</v>
       </c>
       <c r="Q20" s="2" t="s">
@@ -1851,7 +1972,115 @@
         <v>19</v>
       </c>
     </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="15"/>
+      <c r="C27" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="20"/>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>